<commit_message>
Updated Figures + Added Cover Letter + Updated Data Table
</commit_message>
<xml_diff>
--- a/DataTables.xlsx
+++ b/DataTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\FoamFireArticle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB92EB3-A8AF-46F4-8B44-BA1152B24F49}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B84013-5D60-48C5-A077-378F1AD73218}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1398" windowWidth="20640" windowHeight="11520" tabRatio="848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="222" yWindow="198" windowWidth="20778" windowHeight="11916" tabRatio="848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fig13_Retained yield strength" sheetId="8" r:id="rId1"/>
@@ -39,12 +39,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="18">
   <si>
     <t>Densification Strain</t>
-  </si>
-  <si>
-    <t>Energy Absorption Capacity</t>
   </si>
   <si>
     <t>---</t>
@@ -115,13 +112,19 @@
     <t>Retained plateau strength</t>
   </si>
   <si>
-    <t>Retained Quasi-Elastic Modulus</t>
+    <t>NA</t>
   </si>
   <si>
-    <t>Quasi-Hardening Modulus</t>
+    <t>XXX</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>Energy Absorption Capacity (MJ/m^3)</t>
+  </si>
+  <si>
+    <t>Quasi-Hardening Modulus (Mpa)</t>
+  </si>
+  <si>
+    <t>Retained Quasi-Elastic Modulus (Mpa)</t>
   </si>
 </sst>
 </file>
@@ -130,7 +133,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -523,16 +526,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -883,7 +886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
@@ -902,28 +905,28 @@
     <row r="1" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:14" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>4</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>5</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -934,7 +937,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="31">
         <v>150</v>
@@ -957,7 +960,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="32">
         <v>150</v>
@@ -986,7 +989,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="33">
         <v>200</v>
@@ -1006,7 +1009,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="34">
         <v>200</v>
@@ -1035,7 +1038,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="35">
         <v>300</v>
@@ -1058,7 +1061,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="36">
         <v>300</v>
@@ -1081,7 +1084,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="36">
         <v>300</v>
@@ -1104,7 +1107,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="32">
         <v>300</v>
@@ -1140,7 +1143,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="33">
         <v>400</v>
@@ -1160,7 +1163,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="34">
         <v>400</v>
@@ -1189,7 +1192,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="35">
         <v>550</v>
@@ -1209,7 +1212,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" s="36">
         <v>550</v>
@@ -1218,16 +1221,16 @@
         <v>30</v>
       </c>
       <c r="F14" s="77" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G14" s="65" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14" s="65" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="66" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -1235,7 +1238,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="33">
         <v>700</v>
@@ -1255,7 +1258,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" s="34">
         <v>700</v>
@@ -1264,16 +1267,16 @@
         <v>30</v>
       </c>
       <c r="F16" s="73" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G16" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" s="60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -1281,7 +1284,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="36">
         <v>150</v>
@@ -1301,7 +1304,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="32">
         <v>150</v>
@@ -1330,7 +1333,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" s="33">
         <v>200</v>
@@ -1350,7 +1353,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" s="34">
         <v>200</v>
@@ -1379,7 +1382,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="35">
         <v>300</v>
@@ -1399,7 +1402,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" s="32">
         <v>300</v>
@@ -1428,7 +1431,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="33">
         <v>500</v>
@@ -1448,7 +1451,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24" s="34">
         <v>500</v>
@@ -1457,16 +1460,16 @@
         <v>30</v>
       </c>
       <c r="F24" s="73" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G24" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24" s="60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -1514,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1533,28 +1536,28 @@
     <row r="1" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:14" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>4</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>5</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1565,7 +1568,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="31">
         <v>150</v>
@@ -1588,7 +1591,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="32">
         <v>150</v>
@@ -1617,7 +1620,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="33">
         <v>200</v>
@@ -1637,7 +1640,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="34">
         <v>200</v>
@@ -1666,7 +1669,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="35">
         <v>300</v>
@@ -1689,7 +1692,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="36">
         <v>300</v>
@@ -1712,7 +1715,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="36">
         <v>300</v>
@@ -1735,7 +1738,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="32">
         <v>300</v>
@@ -1771,7 +1774,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="33">
         <v>400</v>
@@ -1791,7 +1794,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="34">
         <v>400</v>
@@ -1820,7 +1823,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="35">
         <v>550</v>
@@ -1840,7 +1843,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" s="32">
         <v>550</v>
@@ -1849,16 +1852,16 @@
         <v>30</v>
       </c>
       <c r="F14" s="77" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G14" s="50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14" s="50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="67" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -1866,7 +1869,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="33">
         <v>700</v>
@@ -1886,7 +1889,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" s="34">
         <v>700</v>
@@ -1895,16 +1898,16 @@
         <v>30</v>
       </c>
       <c r="F16" s="73" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G16" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" s="60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -1912,7 +1915,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="35">
         <v>150</v>
@@ -1932,7 +1935,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="32">
         <v>150</v>
@@ -1961,7 +1964,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" s="33">
         <v>200</v>
@@ -1981,7 +1984,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" s="34">
         <v>200</v>
@@ -2010,7 +2013,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="35">
         <v>300</v>
@@ -2030,7 +2033,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" s="32">
         <v>300</v>
@@ -2059,7 +2062,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="33">
         <v>500</v>
@@ -2079,7 +2082,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24" s="34">
         <v>500</v>
@@ -2088,16 +2091,16 @@
         <v>30</v>
       </c>
       <c r="F24" s="73" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G24" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24" s="60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -2123,8 +2126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2142,30 +2145,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:14" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="2:14" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>4</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>5</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -2176,7 +2179,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="31">
         <v>150</v>
@@ -2199,7 +2202,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="36">
         <v>150</v>
@@ -2228,7 +2231,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="33">
         <v>200</v>
@@ -2248,7 +2251,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="34">
         <v>200</v>
@@ -2277,7 +2280,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="35">
         <v>300</v>
@@ -2300,7 +2303,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="36">
         <v>300</v>
@@ -2323,7 +2326,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="36">
         <v>300</v>
@@ -2346,7 +2349,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="32">
         <v>300</v>
@@ -2382,7 +2385,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="33">
         <v>400</v>
@@ -2402,7 +2405,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="34">
         <v>400</v>
@@ -2431,7 +2434,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="35">
         <v>550</v>
@@ -2451,7 +2454,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" s="32">
         <v>550</v>
@@ -2460,16 +2463,16 @@
         <v>30</v>
       </c>
       <c r="F14" s="72" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G14" s="50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14" s="50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="67" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -2477,7 +2480,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="33">
         <v>700</v>
@@ -2497,7 +2500,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" s="34">
         <v>700</v>
@@ -2506,16 +2509,16 @@
         <v>30</v>
       </c>
       <c r="F16" s="73" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G16" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" s="60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -2523,7 +2526,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="36">
         <v>150</v>
@@ -2543,7 +2546,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="36">
         <v>150</v>
@@ -2572,7 +2575,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" s="33">
         <v>200</v>
@@ -2592,7 +2595,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" s="54">
         <v>200</v>
@@ -2621,7 +2624,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="35">
         <v>300</v>
@@ -2641,7 +2644,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" s="32">
         <v>300</v>
@@ -2670,7 +2673,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="54">
         <v>500</v>
@@ -2690,7 +2693,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24" s="34">
         <v>500</v>
@@ -2699,16 +2702,16 @@
         <v>30</v>
       </c>
       <c r="F24" s="73" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G24" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24" s="60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -2734,8 +2737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:N27"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2753,28 +2756,28 @@
     <row r="1" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:14" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>4</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>5</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -2785,7 +2788,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="31">
         <v>150</v>
@@ -2808,7 +2811,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="32">
         <v>150</v>
@@ -2837,7 +2840,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="33">
         <v>200</v>
@@ -2857,7 +2860,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="34">
         <v>200</v>
@@ -2886,7 +2889,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="35">
         <v>300</v>
@@ -2909,7 +2912,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="36">
         <v>300</v>
@@ -2932,7 +2935,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="36">
         <v>300</v>
@@ -2955,7 +2958,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="32">
         <v>300</v>
@@ -2991,7 +2994,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="33">
         <v>400</v>
@@ -3011,7 +3014,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="34">
         <v>400</v>
@@ -3040,7 +3043,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="35">
         <v>550</v>
@@ -3060,7 +3063,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" s="32">
         <v>550</v>
@@ -3069,16 +3072,16 @@
         <v>30</v>
       </c>
       <c r="F14" s="72" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G14" s="50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14" s="50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="67" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -3086,7 +3089,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="33">
         <v>700</v>
@@ -3106,7 +3109,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" s="34">
         <v>700</v>
@@ -3115,16 +3118,16 @@
         <v>30</v>
       </c>
       <c r="F16" s="73" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G16" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" s="60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -3132,7 +3135,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="35">
         <v>150</v>
@@ -3152,7 +3155,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="32">
         <v>150</v>
@@ -3181,7 +3184,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" s="33">
         <v>200</v>
@@ -3201,7 +3204,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" s="34">
         <v>200</v>
@@ -3230,7 +3233,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="35">
         <v>300</v>
@@ -3250,7 +3253,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" s="32">
         <v>300</v>
@@ -3279,7 +3282,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="33">
         <v>500</v>
@@ -3299,7 +3302,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24" s="34">
         <v>500</v>
@@ -3308,16 +3311,16 @@
         <v>30</v>
       </c>
       <c r="F24" s="73" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G24" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24" s="60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -3347,7 +3350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
@@ -3368,28 +3371,28 @@
     <row r="1" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:14" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>4</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>5</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -3400,7 +3403,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="31">
         <v>150</v>
@@ -3423,7 +3426,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="32">
         <v>150</v>
@@ -3452,7 +3455,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="33">
         <v>200</v>
@@ -3472,7 +3475,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="34">
         <v>200</v>
@@ -3501,7 +3504,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="35">
         <v>300</v>
@@ -3524,7 +3527,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="36">
         <v>300</v>
@@ -3547,7 +3550,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="36">
         <v>300</v>
@@ -3570,7 +3573,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="32">
         <v>300</v>
@@ -3606,7 +3609,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="54">
         <v>400</v>
@@ -3626,7 +3629,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="54">
         <v>400</v>
@@ -3655,7 +3658,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="35">
         <v>550</v>
@@ -3675,7 +3678,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" s="32">
         <v>550</v>
@@ -3684,16 +3687,16 @@
         <v>30</v>
       </c>
       <c r="F14" s="72" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G14" s="50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14" s="50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="67" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -3701,7 +3704,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="33">
         <v>700</v>
@@ -3721,7 +3724,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" s="34">
         <v>700</v>
@@ -3730,16 +3733,16 @@
         <v>30</v>
       </c>
       <c r="F16" s="73" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G16" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" s="60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -3747,7 +3750,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="36">
         <v>150</v>
@@ -3767,7 +3770,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="36">
         <v>150</v>
@@ -3796,7 +3799,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" s="33">
         <v>200</v>
@@ -3816,7 +3819,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" s="34">
         <v>200</v>
@@ -3845,7 +3848,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="35">
         <v>300</v>
@@ -3865,7 +3868,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" s="32">
         <v>300</v>
@@ -3894,7 +3897,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="33">
         <v>500</v>
@@ -3914,7 +3917,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24" s="34">
         <v>500</v>
@@ -3923,16 +3926,16 @@
         <v>30</v>
       </c>
       <c r="F24" s="73" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G24" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24" s="60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -3958,8 +3961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="B1:N25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3975,30 +3978,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:14" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="2:14" ht="57.9" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>4</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>5</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -4009,7 +4012,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="31">
         <v>150</v>
@@ -4032,7 +4035,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="36">
         <v>150</v>
@@ -4061,7 +4064,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="33">
         <v>200</v>
@@ -4081,7 +4084,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="34">
         <v>200</v>
@@ -4110,7 +4113,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="35">
         <v>300</v>
@@ -4133,7 +4136,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="36">
         <v>300</v>
@@ -4156,7 +4159,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="36">
         <v>300</v>
@@ -4179,7 +4182,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="32">
         <v>300</v>
@@ -4215,7 +4218,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="33">
         <v>400</v>
@@ -4235,7 +4238,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="34">
         <v>400</v>
@@ -4264,7 +4267,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="35">
         <v>550</v>
@@ -4284,7 +4287,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" s="32">
         <v>550</v>
@@ -4293,16 +4296,16 @@
         <v>30</v>
       </c>
       <c r="F14" s="72" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G14" s="50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14" s="50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="67" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -4310,7 +4313,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="54">
         <v>700</v>
@@ -4330,7 +4333,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" s="34">
         <v>700</v>
@@ -4339,16 +4342,16 @@
         <v>30</v>
       </c>
       <c r="F16" s="73" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G16" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" s="60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -4356,7 +4359,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="35">
         <v>150</v>
@@ -4376,7 +4379,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="32">
         <v>150</v>
@@ -4405,7 +4408,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" s="33">
         <v>200</v>
@@ -4425,7 +4428,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" s="34">
         <v>200</v>
@@ -4454,7 +4457,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="35">
         <v>300</v>
@@ -4474,7 +4477,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" s="32">
         <v>300</v>
@@ -4503,7 +4506,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="54">
         <v>500</v>
@@ -4523,7 +4526,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24" s="34">
         <v>500</v>
@@ -4532,16 +4535,16 @@
         <v>30</v>
       </c>
       <c r="F24" s="73" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G24" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24" s="60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -4560,8 +4563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="B1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4579,28 +4582,28 @@
     <row r="1" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:14" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>4</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>5</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -4611,7 +4614,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="31">
         <v>150</v>
@@ -4634,7 +4637,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="36">
         <v>150</v>
@@ -4663,7 +4666,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="33">
         <v>200</v>
@@ -4683,7 +4686,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="34">
         <v>200</v>
@@ -4712,7 +4715,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="35">
         <v>300</v>
@@ -4735,7 +4738,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="36">
         <v>300</v>
@@ -4758,7 +4761,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="36">
         <v>300</v>
@@ -4781,7 +4784,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="32">
         <v>300</v>
@@ -4817,7 +4820,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="33">
         <v>400</v>
@@ -4837,7 +4840,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="34">
         <v>400</v>
@@ -4866,7 +4869,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="35">
         <v>550</v>
@@ -4886,7 +4889,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" s="32">
         <v>550</v>
@@ -4895,16 +4898,16 @@
         <v>30</v>
       </c>
       <c r="F14" s="72" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G14" s="50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14" s="50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="67" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -4912,7 +4915,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="33">
         <v>700</v>
@@ -4932,7 +4935,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" s="34">
         <v>700</v>
@@ -4941,16 +4944,16 @@
         <v>30</v>
       </c>
       <c r="F16" s="73" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G16" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" s="60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -4958,7 +4961,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="36">
         <v>150</v>
@@ -4978,7 +4981,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="36">
         <v>150</v>
@@ -5007,7 +5010,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" s="33">
         <v>200</v>
@@ -5027,7 +5030,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" s="34">
         <v>200</v>
@@ -5056,7 +5059,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="35">
         <v>300</v>
@@ -5076,7 +5079,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" s="32">
         <v>300</v>
@@ -5084,20 +5087,20 @@
       <c r="E22" s="38">
         <v>30</v>
       </c>
-      <c r="F22" s="72">
-        <v>1.3797406380358299</v>
+      <c r="F22" s="72" t="s">
+        <v>14</v>
       </c>
       <c r="G22" s="20">
         <f>AVERAGE(F21:F22)</f>
-        <v>1.1577196373758794</v>
-      </c>
-      <c r="H22" s="21">
+        <v>0.93569863671592901</v>
+      </c>
+      <c r="H22" s="21" t="e">
         <f>_xlfn.STDEV.S(F21:F22)</f>
-        <v>0.31398511026494841</v>
-      </c>
-      <c r="I22" s="22">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" s="22" t="e">
         <f>H22/G22</f>
-        <v>0.27120997185176549</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -5105,7 +5108,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="33">
         <v>500</v>
@@ -5113,8 +5116,8 @@
       <c r="E23" s="57">
         <v>15</v>
       </c>
-      <c r="F23" s="75">
-        <v>7.9571554635787303</v>
+      <c r="F23" s="75" t="s">
+        <v>14</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -5125,7 +5128,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24" s="34">
         <v>500</v>
@@ -5134,16 +5137,16 @@
         <v>30</v>
       </c>
       <c r="F24" s="73" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G24" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24" s="60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Update the figure 22 and excel file
</commit_message>
<xml_diff>
--- a/DataTables.xlsx
+++ b/DataTables.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\FoamFireArticle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\14a - UNICAMP_ ARTIGOS\PLOTS_MIGUEL TAVARES\09 - LIST OF SYMBOLS\Miguels Paper\IJMS\FoamFireArticle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB92EB3-A8AF-46F4-8B44-BA1152B24F49}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1398" windowWidth="20640" windowHeight="11520" tabRatio="848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1404" windowWidth="20640" windowHeight="11520" tabRatio="848" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Fig13_Retained yield strength" sheetId="8" r:id="rId1"/>
@@ -24,7 +23,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Fig13_Retained yield strength'!$B$2:$H$2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="18">
   <si>
     <t>Densification Strain</t>
   </si>
@@ -123,14 +122,17 @@
   <si>
     <t>NA</t>
   </si>
+  <si>
+    <t>No Sample</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -523,16 +525,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -556,9 +558,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -880,27 +882,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7890625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.89453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.89453125" style="2"/>
-    <col min="4" max="4" width="12.20703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.68359375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.68359375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="7.7890625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.89453125" style="2"/>
+    <col min="1" max="1" width="2.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="12.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="2" customWidth="1"/>
+    <col min="7" max="9" width="7.77734375" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:14" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
@@ -929,7 +931,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -952,7 +954,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -981,7 +983,7 @@
         <v>0.14526797367059971</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -1001,7 +1003,7 @@
       <c r="H5" s="23"/>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -1030,7 +1032,7 @@
         <v>0.20058067779670785</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -1053,7 +1055,7 @@
         <v>0.70091410258713804</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="11">
         <v>6</v>
       </c>
@@ -1076,7 +1078,7 @@
         <v>0.716646736490262</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -1099,7 +1101,7 @@
         <v>0.93876181547316295</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -1135,7 +1137,7 @@
         <v>0.17700211545907407</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="12">
         <v>9</v>
       </c>
@@ -1155,7 +1157,7 @@
       <c r="H11" s="23"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -1184,7 +1186,7 @@
         <v>4.2228227237826051E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -1204,7 +1206,7 @@
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -1230,7 +1232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="12">
         <v>13</v>
       </c>
@@ -1250,7 +1252,7 @@
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="11">
         <v>14</v>
       </c>
@@ -1276,7 +1278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="10">
         <v>15</v>
       </c>
@@ -1296,7 +1298,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="11">
         <v>16</v>
       </c>
@@ -1325,7 +1327,7 @@
         <v>0.31571732154919291</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="12">
         <v>17</v>
       </c>
@@ -1345,7 +1347,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="11">
         <v>18</v>
       </c>
@@ -1374,7 +1376,7 @@
         <v>0.31705499571001966</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="12">
         <v>19</v>
       </c>
@@ -1394,7 +1396,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="11">
         <v>20</v>
       </c>
@@ -1423,7 +1425,7 @@
         <v>4.3899118191247713E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="12">
         <v>21</v>
       </c>
@@ -1443,7 +1445,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="13">
         <v>22</v>
       </c>
@@ -1469,36 +1471,36 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D25" s="45"/>
       <c r="E25" s="46"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D26" s="45"/>
       <c r="E26" s="46"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D27" s="45"/>
       <c r="E27" s="46"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D28" s="45"/>
       <c r="E28" s="46"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D29" s="45"/>
       <c r="E29" s="46"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D30" s="45"/>
       <c r="E30" s="46"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D31" s="45"/>
       <c r="E31" s="45"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:H2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B2:H2"/>
   <sortState ref="M7:M10">
     <sortCondition ref="M7"/>
   </sortState>
@@ -1511,27 +1513,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N26"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7890625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.89453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.89453125" style="2"/>
-    <col min="4" max="4" width="12.20703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.68359375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.68359375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="7.7890625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.89453125" style="2"/>
+    <col min="1" max="1" width="2.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="12.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="2" customWidth="1"/>
+    <col min="7" max="9" width="7.77734375" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:14" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
@@ -1560,7 +1562,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -1583,7 +1585,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -1612,7 +1614,7 @@
         <v>2.1097121602629994E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -1632,7 +1634,7 @@
       <c r="H5" s="23"/>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -1661,7 +1663,7 @@
         <v>8.8464473513554919E-3</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -1684,7 +1686,7 @@
         <v>0.97574498583067903</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="11">
         <v>6</v>
       </c>
@@ -1707,7 +1709,7 @@
         <v>0.982973868918111</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -1730,7 +1732,7 @@
         <v>1.0029047145410499</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -1766,7 +1768,7 @@
         <v>1.6307637007625678E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="12">
         <v>9</v>
       </c>
@@ -1786,7 +1788,7 @@
       <c r="H11" s="23"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -1815,7 +1817,7 @@
         <v>7.1010789428390363E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -1835,7 +1837,7 @@
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -1861,7 +1863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="12">
         <v>13</v>
       </c>
@@ -1881,7 +1883,7 @@
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="11">
         <v>14</v>
       </c>
@@ -1907,7 +1909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="10">
         <v>15</v>
       </c>
@@ -1927,7 +1929,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="11">
         <v>16</v>
       </c>
@@ -1956,7 +1958,7 @@
         <v>0.14756083996496799</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="12">
         <v>17</v>
       </c>
@@ -1976,7 +1978,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="11">
         <v>18</v>
       </c>
@@ -2005,7 +2007,7 @@
         <v>0.34756964057331874</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="12">
         <v>19</v>
       </c>
@@ -2025,7 +2027,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="11">
         <v>20</v>
       </c>
@@ -2054,7 +2056,7 @@
         <v>0.18288637106314115</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="12">
         <v>21</v>
       </c>
@@ -2074,7 +2076,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="13">
         <v>22</v>
       </c>
@@ -2100,11 +2102,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D25" s="45"/>
       <c r="E25" s="46"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D26" s="45"/>
       <c r="E26" s="46"/>
     </row>
@@ -2120,29 +2122,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N26"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7890625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.89453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.89453125" style="2"/>
-    <col min="4" max="4" width="12.20703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.68359375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.68359375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="7.7890625" style="2" customWidth="1"/>
-    <col min="10" max="12" width="8.89453125" style="2"/>
-    <col min="13" max="13" width="9.41796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.89453125" style="2"/>
+    <col min="1" max="1" width="2.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="12.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="2" customWidth="1"/>
+    <col min="7" max="9" width="7.77734375" style="2" customWidth="1"/>
+    <col min="10" max="12" width="8.88671875" style="2"/>
+    <col min="13" max="13" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:14" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
@@ -2171,7 +2173,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -2194,7 +2196,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -2223,7 +2225,7 @@
         <v>4.7385356839080489E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -2243,7 +2245,7 @@
       <c r="H5" s="23"/>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -2272,7 +2274,7 @@
         <v>6.7531948824370955E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -2295,7 +2297,7 @@
         <v>1.19569788305308</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="11">
         <v>6</v>
       </c>
@@ -2318,7 +2320,7 @@
         <v>1.2194359121409899</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -2341,7 +2343,7 @@
         <v>1.77425529643583</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -2377,7 +2379,7 @@
         <v>0.44994519564122748</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="12">
         <v>9</v>
       </c>
@@ -2397,7 +2399,7 @@
       <c r="H11" s="23"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -2426,7 +2428,7 @@
         <v>6.3368647725771346E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -2446,7 +2448,7 @@
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -2472,7 +2474,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="12">
         <v>13</v>
       </c>
@@ -2492,7 +2494,7 @@
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="11">
         <v>14</v>
       </c>
@@ -2518,7 +2520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="10">
         <v>15</v>
       </c>
@@ -2538,7 +2540,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="11">
         <v>16</v>
       </c>
@@ -2567,7 +2569,7 @@
         <v>0.53969646527891901</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="12">
         <v>17</v>
       </c>
@@ -2587,7 +2589,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="11">
         <v>18</v>
       </c>
@@ -2616,7 +2618,7 @@
         <v>0.44134662364904237</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="12">
         <v>19</v>
       </c>
@@ -2636,7 +2638,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="11">
         <v>20</v>
       </c>
@@ -2665,7 +2667,7 @@
         <v>0.16660236033646106</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="12">
         <v>21</v>
       </c>
@@ -2685,7 +2687,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="13">
         <v>22</v>
       </c>
@@ -2711,11 +2713,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D25" s="45"/>
       <c r="E25" s="46"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D26" s="45"/>
       <c r="E26" s="46"/>
     </row>
@@ -2731,27 +2733,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N27"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7890625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.89453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.89453125" style="2"/>
-    <col min="4" max="4" width="12.20703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.68359375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.68359375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="7.7890625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.89453125" style="2"/>
+    <col min="1" max="1" width="2.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="12.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="2" customWidth="1"/>
+    <col min="7" max="9" width="7.77734375" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:14" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
@@ -2780,7 +2782,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -2803,7 +2805,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -2832,7 +2834,7 @@
         <v>2.6826977033976924E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -2852,7 +2854,7 @@
       <c r="H5" s="23"/>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -2881,7 +2883,7 @@
         <v>0.22903088985525652</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -2904,7 +2906,7 @@
         <v>5.70671799511498</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="11">
         <v>6</v>
       </c>
@@ -2927,7 +2929,7 @@
         <v>6.5621740368524604</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -2950,7 +2952,7 @@
         <v>8.12727339067294</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -2986,7 +2988,7 @@
         <v>0.17919322511738361</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="12">
         <v>9</v>
       </c>
@@ -3006,7 +3008,7 @@
       <c r="H11" s="23"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -3035,7 +3037,7 @@
         <v>2.3714081726065751E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -3055,7 +3057,7 @@
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -3081,7 +3083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="12">
         <v>13</v>
       </c>
@@ -3101,7 +3103,7 @@
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="11">
         <v>14</v>
       </c>
@@ -3127,7 +3129,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="10">
         <v>15</v>
       </c>
@@ -3147,7 +3149,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="11">
         <v>16</v>
       </c>
@@ -3176,7 +3178,7 @@
         <v>4.4745319054174133E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="12">
         <v>17</v>
       </c>
@@ -3196,7 +3198,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="11">
         <v>18</v>
       </c>
@@ -3225,7 +3227,7 @@
         <v>0.62012006327318359</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="12">
         <v>19</v>
       </c>
@@ -3245,7 +3247,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="11">
         <v>20</v>
       </c>
@@ -3274,7 +3276,7 @@
         <v>1.2101659242331178</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="12">
         <v>21</v>
       </c>
@@ -3294,7 +3296,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="13">
         <v>22</v>
       </c>
@@ -3320,15 +3322,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D25" s="45"/>
       <c r="E25" s="46"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D26" s="45"/>
       <c r="E26" s="46"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D27" s="45"/>
       <c r="E27" s="46"/>
     </row>
@@ -3344,29 +3346,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N26"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7890625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.89453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.89453125" style="2"/>
-    <col min="4" max="4" width="12.20703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.68359375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.68359375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="7.7890625" style="2" customWidth="1"/>
-    <col min="10" max="12" width="8.89453125" style="2"/>
-    <col min="13" max="13" width="9.41796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.89453125" style="2"/>
+    <col min="1" max="1" width="2.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="12.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="2" customWidth="1"/>
+    <col min="7" max="9" width="7.77734375" style="2" customWidth="1"/>
+    <col min="10" max="12" width="8.88671875" style="2"/>
+    <col min="13" max="13" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:14" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
@@ -3395,7 +3397,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -3418,7 +3420,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -3447,7 +3449,7 @@
         <v>5.677872490308309E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -3467,7 +3469,7 @@
       <c r="H5" s="23"/>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -3496,7 +3498,7 @@
         <v>2.0710078574284849E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -3519,7 +3521,7 @@
         <v>0.37378688770538299</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="11">
         <v>6</v>
       </c>
@@ -3542,7 +3544,7 @@
         <v>0.38037299526942198</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -3565,7 +3567,7 @@
         <v>0.384164974612001</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -3601,7 +3603,7 @@
         <v>2.7142022318979806E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="12">
         <v>9</v>
       </c>
@@ -3621,7 +3623,7 @@
       <c r="H11" s="52"/>
       <c r="I11" s="53"/>
     </row>
-    <row r="12" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -3650,7 +3652,7 @@
         <v>4.4330140470684428E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -3670,7 +3672,7 @@
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -3696,7 +3698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="12">
         <v>13</v>
       </c>
@@ -3716,7 +3718,7 @@
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="11">
         <v>14</v>
       </c>
@@ -3742,7 +3744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="10">
         <v>15</v>
       </c>
@@ -3762,7 +3764,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="11">
         <v>16</v>
       </c>
@@ -3791,7 +3793,7 @@
         <v>1.0477881543035028E-4</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="12">
         <v>17</v>
       </c>
@@ -3811,7 +3813,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="11">
         <v>18</v>
       </c>
@@ -3840,7 +3842,7 @@
         <v>0.25115875540211463</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="12">
         <v>19</v>
       </c>
@@ -3860,7 +3862,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="11">
         <v>20</v>
       </c>
@@ -3889,7 +3891,7 @@
         <v>0.25153107170162187</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="12">
         <v>21</v>
       </c>
@@ -3909,7 +3911,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="13">
         <v>22</v>
       </c>
@@ -3935,11 +3937,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D25" s="45"/>
       <c r="E25" s="46"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D26" s="45"/>
       <c r="E26" s="46"/>
     </row>
@@ -3955,27 +3957,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N25"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7890625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.89453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.89453125" style="2"/>
-    <col min="4" max="4" width="12.20703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.68359375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.68359375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="7.7890625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.89453125" style="2"/>
+    <col min="1" max="1" width="2.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="12.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="2" customWidth="1"/>
+    <col min="7" max="9" width="7.77734375" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:14" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:14" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
@@ -4004,7 +4006,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -4027,7 +4029,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -4056,7 +4058,7 @@
         <v>2.8936379508679045E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -4076,7 +4078,7 @@
       <c r="H5" s="23"/>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -4105,7 +4107,7 @@
         <v>2.0333104078973579E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -4128,7 +4130,7 @@
         <v>5.4147152806680898</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="11">
         <v>6</v>
       </c>
@@ -4151,7 +4153,7 @@
         <v>5.3848833614323004</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -4174,7 +4176,7 @@
         <v>5.3219131078384603</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -4210,7 +4212,7 @@
         <v>1.4411452912174955E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="12">
         <v>9</v>
       </c>
@@ -4230,7 +4232,7 @@
       <c r="H11" s="23"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -4259,7 +4261,7 @@
         <v>5.883428730232571E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -4279,7 +4281,7 @@
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -4305,7 +4307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="12">
         <v>13</v>
       </c>
@@ -4325,7 +4327,7 @@
       <c r="H15" s="52"/>
       <c r="I15" s="53"/>
     </row>
-    <row r="16" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="11">
         <v>14</v>
       </c>
@@ -4351,7 +4353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="10">
         <v>15</v>
       </c>
@@ -4371,7 +4373,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="11">
         <v>16</v>
       </c>
@@ -4400,7 +4402,7 @@
         <v>0.2231149399793004</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="12">
         <v>17</v>
       </c>
@@ -4420,7 +4422,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="11">
         <v>18</v>
       </c>
@@ -4449,7 +4451,7 @@
         <v>0.35228114987052844</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="12">
         <v>19</v>
       </c>
@@ -4469,7 +4471,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="11">
         <v>20</v>
       </c>
@@ -4498,7 +4500,7 @@
         <v>0.1593216771454497</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="12">
         <v>21</v>
       </c>
@@ -4518,7 +4520,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="13">
         <v>22</v>
       </c>
@@ -4544,7 +4546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D25" s="45"/>
       <c r="E25" s="46"/>
     </row>
@@ -4557,27 +4559,27 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7:M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7890625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.89453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.89453125" style="2"/>
-    <col min="4" max="4" width="12.20703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.68359375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.68359375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="7.7890625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.89453125" style="2"/>
+    <col min="1" max="1" width="2.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="12.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="2" customWidth="1"/>
+    <col min="7" max="9" width="7.77734375" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:14" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
@@ -4606,7 +4608,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -4620,7 +4622,7 @@
         <v>15</v>
       </c>
       <c r="F3" s="74">
-        <v>0.76190421914561801</v>
+        <v>0.76186897132864095</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
@@ -4629,7 +4631,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -4643,22 +4645,22 @@
         <v>30</v>
       </c>
       <c r="F4" s="74">
-        <v>0.78525788766120697</v>
+        <v>0.78514709098936497</v>
       </c>
       <c r="G4" s="55">
         <f>AVERAGE(F3:F4)</f>
-        <v>0.77358105340341243</v>
+        <v>0.77350803115900302</v>
       </c>
       <c r="H4" s="56">
         <f>_xlfn.STDEV.S(F3:F4)</f>
-        <v>1.6513537372955724E-2</v>
+        <v>1.6460116265369848E-2</v>
       </c>
       <c r="I4" s="64">
         <f>H4/G4</f>
-        <v>2.1346874125605205E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+        <v>2.1279825938854784E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -4672,13 +4674,13 @@
         <v>15</v>
       </c>
       <c r="F5" s="75">
-        <v>0.79065587810255</v>
+        <v>0.79522786376675303</v>
       </c>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -4692,22 +4694,22 @@
         <v>30</v>
       </c>
       <c r="F6" s="73">
-        <v>0.79009101790394498</v>
+        <v>0.78982757506022905</v>
       </c>
       <c r="G6" s="25">
         <f>AVERAGE(F5:F6)</f>
-        <v>0.79037344800324749</v>
+        <v>0.79252771941349098</v>
       </c>
       <c r="H6" s="26">
         <f>_xlfn.STDEV.S(F5:F6)</f>
-        <v>3.9941647685599082E-4</v>
+        <v>3.8185807647482368E-3</v>
       </c>
       <c r="I6" s="27">
         <f>H6/G6</f>
-        <v>5.0535158774001434E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+        <v>4.8182299132378259E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -4721,16 +4723,16 @@
         <v>15</v>
       </c>
       <c r="F7" s="76">
-        <v>0.80980838767651298</v>
+        <v>0.81142827210842305</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="24"/>
-      <c r="M7" s="68">
-        <v>0.77528006835879903</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M7" s="76">
+        <v>0.81142827200000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="11">
         <v>6</v>
       </c>
@@ -4744,16 +4746,16 @@
         <v>30</v>
       </c>
       <c r="F8" s="77">
-        <v>0.77528006835879903</v>
+        <v>0.77528859277047801</v>
       </c>
       <c r="G8" s="28"/>
       <c r="H8" s="29"/>
       <c r="I8" s="30"/>
-      <c r="M8" s="69">
-        <v>0.80980838767651298</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M8" s="77">
+        <v>0.77528859299999997</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -4767,16 +4769,16 @@
         <v>15</v>
       </c>
       <c r="F9" s="77">
-        <v>0.85062669099685995</v>
+        <v>0.850827072994217</v>
       </c>
       <c r="G9" s="28"/>
       <c r="H9" s="29"/>
       <c r="I9" s="30"/>
-      <c r="M9" s="69">
-        <v>0.821221003647154</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="M9" s="77">
+        <v>0.85082707300000004</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -4790,29 +4792,29 @@
         <v>30</v>
       </c>
       <c r="F10" s="72">
-        <v>0.821221003647154</v>
+        <v>0.82117144427272404</v>
       </c>
       <c r="G10" s="20">
         <f>AVERAGE(F7:F10)</f>
-        <v>0.81423403766983149</v>
+        <v>0.81467884553646053</v>
       </c>
       <c r="H10" s="21">
         <f>_xlfn.STDEV.S(F7:F10)</f>
-        <v>3.114611271998351E-2</v>
+        <v>3.1150208277885217E-2</v>
       </c>
       <c r="I10" s="22">
         <f>H10/G10</f>
-        <v>3.8252039682739387E-2</v>
-      </c>
-      <c r="M10" s="70">
-        <v>0.85062669099685995</v>
+        <v>3.8236181592972401E-2</v>
+      </c>
+      <c r="M10" s="72">
+        <v>0.82117144399999997</v>
       </c>
       <c r="N10" s="71">
         <f>I10</f>
-        <v>3.8252039682739387E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+        <v>3.8236181592972401E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="12">
         <v>9</v>
       </c>
@@ -4826,13 +4828,13 @@
         <v>15</v>
       </c>
       <c r="F11" s="75">
-        <v>0.74991939583480105</v>
+        <v>0.74996612541989005</v>
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -4846,22 +4848,22 @@
         <v>30</v>
       </c>
       <c r="F12" s="73">
-        <v>0.76313315118429903</v>
+        <v>0.76237080581552596</v>
       </c>
       <c r="G12" s="25">
         <f>AVERAGE(F11:F12)</f>
-        <v>0.75652627350955004</v>
+        <v>0.75616846561770801</v>
       </c>
       <c r="H12" s="26">
         <f>_xlfn.STDEV.S(F11:F12)</f>
-        <v>9.34353601257004E-3</v>
+        <v>8.7714336262059798E-3</v>
       </c>
       <c r="I12" s="27">
         <f>H12/G12</f>
-        <v>1.2350577025203728E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+        <v>1.1599840544845606E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -4875,13 +4877,13 @@
         <v>15</v>
       </c>
       <c r="F13" s="76">
-        <v>0.72826333252823405</v>
+        <v>0.72943610951139104</v>
       </c>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -4895,7 +4897,7 @@
         <v>30</v>
       </c>
       <c r="F14" s="72" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G14" s="50" t="s">
         <v>2</v>
@@ -4907,7 +4909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="12">
         <v>13</v>
       </c>
@@ -4921,13 +4923,13 @@
         <v>15</v>
       </c>
       <c r="F15" s="75">
-        <v>0.82108068494353004</v>
+        <v>0.82088178902345099</v>
       </c>
       <c r="G15" s="23"/>
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="11">
         <v>14</v>
       </c>
@@ -4941,7 +4943,7 @@
         <v>30</v>
       </c>
       <c r="F16" s="73" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G16" s="58" t="s">
         <v>2</v>
@@ -4953,7 +4955,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="10">
         <v>15</v>
       </c>
@@ -4967,13 +4969,13 @@
         <v>15</v>
       </c>
       <c r="F17" s="74">
-        <v>0.66366487750727299</v>
+        <v>0.75261688024566598</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="11">
         <v>16</v>
       </c>
@@ -4987,22 +4989,22 @@
         <v>30</v>
       </c>
       <c r="F18" s="74">
-        <v>0.54675479548348904</v>
+        <v>0.79435293357597203</v>
       </c>
       <c r="G18" s="55">
         <f>AVERAGE(F17:F18)</f>
-        <v>0.60520983649538107</v>
+        <v>0.77348490691081895</v>
       </c>
       <c r="H18" s="56">
         <f>_xlfn.STDEV.S(F17:F18)</f>
-        <v>8.2667911788093115E-2</v>
+        <v>2.9511846329822802E-2</v>
       </c>
       <c r="I18" s="64">
         <f>H18/G18</f>
-        <v>0.13659380070027008</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+        <v>3.8154391981207014E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="12">
         <v>17</v>
       </c>
@@ -5016,13 +5018,13 @@
         <v>15</v>
       </c>
       <c r="F19" s="75">
-        <v>1.00363550764458</v>
+        <v>0.94578732603498405</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="11">
         <v>18</v>
       </c>
@@ -5036,22 +5038,22 @@
         <v>30</v>
       </c>
       <c r="F20" s="73">
-        <v>0.55745560831062801</v>
+        <v>0.968625246038328</v>
       </c>
       <c r="G20" s="25">
         <f>AVERAGE(F19:F20)</f>
-        <v>0.78054555797760394</v>
+        <v>0.95720628603665603</v>
       </c>
       <c r="H20" s="26">
         <f>_xlfn.STDEV.S(F19:F20)</f>
-        <v>0.3154968324481689</v>
+        <v>1.6148848102560405E-2</v>
       </c>
       <c r="I20" s="27">
         <f>H20/G20</f>
-        <v>0.40420040729668899</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+        <v>1.6870812841634417E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="12">
         <v>19</v>
       </c>
@@ -5065,13 +5067,13 @@
         <v>15</v>
       </c>
       <c r="F21" s="76">
-        <v>0.93569863671592901</v>
+        <v>0.78454965510937802</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="11">
         <v>20</v>
       </c>
@@ -5085,22 +5087,22 @@
         <v>30</v>
       </c>
       <c r="F22" s="72">
-        <v>1.3797406380358299</v>
+        <v>0.97492797526238795</v>
       </c>
       <c r="G22" s="20">
         <f>AVERAGE(F21:F22)</f>
-        <v>1.1577196373758794</v>
+        <v>0.87973881518588293</v>
       </c>
       <c r="H22" s="21">
         <f>_xlfn.STDEV.S(F21:F22)</f>
-        <v>0.31398511026494841</v>
+        <v>0.13461780117109776</v>
       </c>
       <c r="I22" s="22">
         <f>H22/G22</f>
-        <v>0.27120997185176549</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+        <v>0.15302019059219743</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="12">
         <v>21</v>
       </c>
@@ -5114,13 +5116,13 @@
         <v>15</v>
       </c>
       <c r="F23" s="75">
-        <v>7.9571554635787303</v>
+        <v>0.962410634731658</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="13">
         <v>22</v>
       </c>
@@ -5134,7 +5136,7 @@
         <v>30</v>
       </c>
       <c r="F24" s="73" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G24" s="58" t="s">
         <v>2</v>
@@ -5146,11 +5148,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D25" s="45"/>
       <c r="E25" s="46"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D26" s="45"/>
       <c r="E26" s="46"/>
     </row>

</xml_diff>

<commit_message>
Author Statement + Data Tables
</commit_message>
<xml_diff>
--- a/DataTables.xlsx
+++ b/DataTables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\14a - UNICAMP_ ARTIGOS\PLOTS_MIGUEL TAVARES\09 - LIST OF SYMBOLS\Miguels Paper\IJMS\FoamFireArticle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\FoamFireArticle\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BC14D6-3693-4852-9DB3-0F4B87EA5722}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="848" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="1044" windowWidth="20778" windowHeight="11916" tabRatio="848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fig13_Retained yield strength" sheetId="8" r:id="rId1"/>
@@ -23,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Fig13_Retained yield strength'!$B$2:$H$2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -129,10 +130,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -163,7 +163,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,12 +191,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF66FF33"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -332,7 +326,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -525,16 +519,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -558,9 +542,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
-    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -882,27 +866,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:O31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6:O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="2"/>
-    <col min="4" max="4" width="12.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="2" customWidth="1"/>
-    <col min="7" max="9" width="7.77734375" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="2.7890625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.89453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.89453125" style="2"/>
+    <col min="4" max="4" width="12.20703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.68359375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.68359375" style="2" customWidth="1"/>
+    <col min="7" max="9" width="7.7890625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.89453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="2:15" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
@@ -931,7 +915,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -944,7 +928,7 @@
       <c r="E3" s="37">
         <v>15</v>
       </c>
-      <c r="F3" s="76">
+      <c r="F3" s="72">
         <v>0.72803548690058195</v>
       </c>
       <c r="G3" s="18"/>
@@ -954,7 +938,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -967,7 +951,7 @@
       <c r="E4" s="38">
         <v>30</v>
       </c>
-      <c r="F4" s="72">
+      <c r="F4" s="68">
         <v>0.89472543938384996</v>
       </c>
       <c r="G4" s="20">
@@ -983,7 +967,7 @@
         <v>0.14526797367059971</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -996,14 +980,14 @@
       <c r="E5" s="39">
         <v>15</v>
       </c>
-      <c r="F5" s="75">
+      <c r="F5" s="71">
         <v>0.68722122137202002</v>
       </c>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -1016,7 +1000,7 @@
       <c r="E6" s="40">
         <v>30</v>
       </c>
-      <c r="F6" s="73">
+      <c r="F6" s="69">
         <v>0.91437936800908104</v>
       </c>
       <c r="G6" s="25">
@@ -1031,8 +1015,12 @@
         <f>H6/G6</f>
         <v>0.20058067779670785</v>
       </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -1045,17 +1033,18 @@
       <c r="E7" s="41">
         <v>15</v>
       </c>
-      <c r="F7" s="76">
+      <c r="F7" s="72">
         <v>0.716646736490262</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="24"/>
-      <c r="M7" s="68">
-        <v>0.70091410258713804</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="11">
         <v>6</v>
       </c>
@@ -1068,17 +1057,18 @@
       <c r="E8" s="42">
         <v>30</v>
       </c>
-      <c r="F8" s="77">
+      <c r="F8" s="73">
         <v>0.70091410258713804</v>
       </c>
       <c r="G8" s="28"/>
       <c r="H8" s="29"/>
       <c r="I8" s="30"/>
-      <c r="M8" s="69">
-        <v>0.716646736490262</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -1091,17 +1081,18 @@
       <c r="E9" s="42">
         <v>15</v>
       </c>
-      <c r="F9" s="77">
+      <c r="F9" s="73">
         <v>0.93876181547316295</v>
       </c>
       <c r="G9" s="28"/>
       <c r="H9" s="29"/>
       <c r="I9" s="30"/>
-      <c r="M9" s="69">
-        <v>0.93876181547316295</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -1114,7 +1105,7 @@
       <c r="E10" s="38">
         <v>30</v>
       </c>
-      <c r="F10" s="72">
+      <c r="F10" s="68">
         <v>0.98626793642328303</v>
       </c>
       <c r="G10" s="20">
@@ -1129,15 +1120,12 @@
         <f>H10/G10</f>
         <v>0.17700211545907407</v>
       </c>
-      <c r="M10" s="70">
-        <v>0.98626793642328303</v>
-      </c>
-      <c r="N10" s="71">
-        <f>I10</f>
-        <v>0.17700211545907407</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="12">
         <v>9</v>
       </c>
@@ -1150,14 +1138,18 @@
       <c r="E11" s="39">
         <v>15</v>
       </c>
-      <c r="F11" s="75">
+      <c r="F11" s="71">
         <v>0.86631856840746901</v>
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
       <c r="I11" s="24"/>
-    </row>
-    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -1170,7 +1162,7 @@
       <c r="E12" s="40">
         <v>30</v>
       </c>
-      <c r="F12" s="73">
+      <c r="F12" s="69">
         <v>0.81608230407062698</v>
       </c>
       <c r="G12" s="25">
@@ -1186,7 +1178,7 @@
         <v>4.2228227237826051E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -1199,14 +1191,14 @@
       <c r="E13" s="41">
         <v>15</v>
       </c>
-      <c r="F13" s="76">
+      <c r="F13" s="72">
         <v>0.64695426314210602</v>
       </c>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -1219,7 +1211,7 @@
       <c r="E14" s="51">
         <v>30</v>
       </c>
-      <c r="F14" s="77" t="s">
+      <c r="F14" s="73" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="65" t="s">
@@ -1232,7 +1224,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="12">
         <v>13</v>
       </c>
@@ -1245,14 +1237,14 @@
       <c r="E15" s="39">
         <v>15</v>
       </c>
-      <c r="F15" s="75">
+      <c r="F15" s="71">
         <v>0.28639438289331698</v>
       </c>
       <c r="G15" s="23"/>
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B16" s="11">
         <v>14</v>
       </c>
@@ -1265,7 +1257,7 @@
       <c r="E16" s="59">
         <v>30</v>
       </c>
-      <c r="F16" s="73" t="s">
+      <c r="F16" s="69" t="s">
         <v>16</v>
       </c>
       <c r="G16" s="58" t="s">
@@ -1278,7 +1270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="10">
         <v>15</v>
       </c>
@@ -1291,14 +1283,14 @@
       <c r="E17" s="51">
         <v>15</v>
       </c>
-      <c r="F17" s="77">
+      <c r="F17" s="73">
         <v>0.29548944118265102</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B18" s="11">
         <v>16</v>
       </c>
@@ -1311,7 +1303,7 @@
       <c r="E18" s="38">
         <v>30</v>
       </c>
-      <c r="F18" s="74">
+      <c r="F18" s="70">
         <v>0.46534188391160097</v>
       </c>
       <c r="G18" s="20">
@@ -1327,7 +1319,7 @@
         <v>0.31571732154919291</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="12">
         <v>17</v>
       </c>
@@ -1340,14 +1332,14 @@
       <c r="E19" s="57">
         <v>15</v>
       </c>
-      <c r="F19" s="75">
+      <c r="F19" s="71">
         <v>0.35400039428746799</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B20" s="11">
         <v>18</v>
       </c>
@@ -1360,7 +1352,7 @@
       <c r="E20" s="40">
         <v>30</v>
       </c>
-      <c r="F20" s="73">
+      <c r="F20" s="69">
         <v>0.55859724455592197</v>
       </c>
       <c r="G20" s="25">
@@ -1376,7 +1368,7 @@
         <v>0.31705499571001966</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="12">
         <v>19</v>
       </c>
@@ -1389,14 +1381,14 @@
       <c r="E21" s="41">
         <v>15</v>
       </c>
-      <c r="F21" s="76">
+      <c r="F21" s="72">
         <v>0.27070681970292798</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B22" s="11">
         <v>20</v>
       </c>
@@ -1409,7 +1401,7 @@
       <c r="E22" s="38">
         <v>30</v>
       </c>
-      <c r="F22" s="72">
+      <c r="F22" s="68">
         <v>0.28805143826660501</v>
       </c>
       <c r="G22" s="20">
@@ -1425,7 +1417,7 @@
         <v>4.3899118191247713E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="12">
         <v>21</v>
       </c>
@@ -1438,14 +1430,14 @@
       <c r="E23" s="57">
         <v>15</v>
       </c>
-      <c r="F23" s="75">
+      <c r="F23" s="71">
         <v>4.3748562840551002E-2</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B24" s="13">
         <v>22</v>
       </c>
@@ -1458,7 +1450,7 @@
       <c r="E24" s="40">
         <v>30</v>
       </c>
-      <c r="F24" s="73" t="s">
+      <c r="F24" s="69" t="s">
         <v>16</v>
       </c>
       <c r="G24" s="58" t="s">
@@ -1471,36 +1463,36 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D25" s="45"/>
       <c r="E25" s="46"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D26" s="45"/>
       <c r="E26" s="46"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D27" s="45"/>
       <c r="E27" s="46"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D28" s="45"/>
       <c r="E28" s="46"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D29" s="45"/>
       <c r="E29" s="46"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D30" s="45"/>
       <c r="E30" s="46"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D31" s="45"/>
       <c r="E31" s="45"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:H2"/>
+  <autoFilter ref="B2:H2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState ref="M7:M10">
     <sortCondition ref="M7"/>
   </sortState>
@@ -1513,27 +1505,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B1:P26"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="L6" sqref="L6:P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="2"/>
-    <col min="4" max="4" width="12.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="2" customWidth="1"/>
-    <col min="7" max="9" width="7.77734375" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="2.7890625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.89453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.89453125" style="2"/>
+    <col min="4" max="4" width="12.20703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.68359375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.68359375" style="2" customWidth="1"/>
+    <col min="7" max="9" width="7.7890625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.89453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="2:16" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
@@ -1562,7 +1554,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -1575,7 +1567,7 @@
       <c r="E3" s="37">
         <v>15</v>
       </c>
-      <c r="F3" s="76">
+      <c r="F3" s="72">
         <v>0.90597973773304397</v>
       </c>
       <c r="G3" s="18"/>
@@ -1585,7 +1577,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -1598,7 +1590,7 @@
       <c r="E4" s="38">
         <v>30</v>
       </c>
-      <c r="F4" s="72">
+      <c r="F4" s="68">
         <v>0.93341974796779803</v>
       </c>
       <c r="G4" s="20">
@@ -1614,7 +1606,7 @@
         <v>2.1097121602629994E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -1627,14 +1619,14 @@
       <c r="E5" s="39">
         <v>15</v>
       </c>
-      <c r="F5" s="75">
+      <c r="F5" s="71">
         <v>0.89450474306091399</v>
       </c>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -1647,7 +1639,7 @@
       <c r="E6" s="40">
         <v>30</v>
       </c>
-      <c r="F6" s="73">
+      <c r="F6" s="69">
         <v>0.90576612669575696</v>
       </c>
       <c r="G6" s="25">
@@ -1662,8 +1654,13 @@
         <f>H6/G6</f>
         <v>8.8464473513554919E-3</v>
       </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -1676,17 +1673,19 @@
       <c r="E7" s="41">
         <v>15</v>
       </c>
-      <c r="F7" s="76">
+      <c r="F7" s="72">
         <v>1.0029047145410499</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="24"/>
-      <c r="M7" s="68">
-        <v>0.97574498583067903</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="11">
         <v>6</v>
       </c>
@@ -1699,17 +1698,19 @@
       <c r="E8" s="42">
         <v>30</v>
       </c>
-      <c r="F8" s="77">
+      <c r="F8" s="73">
         <v>1.01003580419107</v>
       </c>
       <c r="G8" s="28"/>
       <c r="H8" s="29"/>
       <c r="I8" s="30"/>
-      <c r="M8" s="69">
-        <v>0.982973868918111</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -1722,17 +1723,19 @@
       <c r="E9" s="42">
         <v>15</v>
       </c>
-      <c r="F9" s="77">
+      <c r="F9" s="73">
         <v>0.982973868918111</v>
       </c>
       <c r="G9" s="28"/>
       <c r="H9" s="29"/>
       <c r="I9" s="30"/>
-      <c r="M9" s="69">
-        <v>1.0029047145410499</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="2:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -1745,7 +1748,7 @@
       <c r="E10" s="38">
         <v>30</v>
       </c>
-      <c r="F10" s="72">
+      <c r="F10" s="68">
         <v>0.97574498583067903</v>
       </c>
       <c r="G10" s="20">
@@ -1760,15 +1763,13 @@
         <f>H10/G10</f>
         <v>1.6307637007625678E-2</v>
       </c>
-      <c r="M10" s="70">
-        <v>1.01003580419107</v>
-      </c>
-      <c r="N10" s="71">
-        <f>I10</f>
-        <v>1.6307637007625678E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="12">
         <v>9</v>
       </c>
@@ -1781,14 +1782,19 @@
       <c r="E11" s="39">
         <v>15</v>
       </c>
-      <c r="F11" s="75">
+      <c r="F11" s="71">
         <v>0.963935769034441</v>
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
       <c r="I11" s="24"/>
-    </row>
-    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="2:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -1801,7 +1807,7 @@
       <c r="E12" s="40">
         <v>30</v>
       </c>
-      <c r="F12" s="73">
+      <c r="F12" s="69">
         <v>0.973664890298511</v>
       </c>
       <c r="G12" s="25">
@@ -1816,8 +1822,13 @@
         <f>H12/G12</f>
         <v>7.1010789428390363E-3</v>
       </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -1830,14 +1841,19 @@
       <c r="E13" s="41">
         <v>15</v>
       </c>
-      <c r="F13" s="76">
+      <c r="F13" s="72">
         <v>0.66160792293853798</v>
       </c>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
-    </row>
-    <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="2:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -1850,7 +1866,7 @@
       <c r="E14" s="43">
         <v>30</v>
       </c>
-      <c r="F14" s="77" t="s">
+      <c r="F14" s="73" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="50" t="s">
@@ -1863,7 +1879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="12">
         <v>13</v>
       </c>
@@ -1876,14 +1892,14 @@
       <c r="E15" s="39">
         <v>15</v>
       </c>
-      <c r="F15" s="75">
+      <c r="F15" s="71">
         <v>0.24168132734574699</v>
       </c>
       <c r="G15" s="23"/>
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B16" s="11">
         <v>14</v>
       </c>
@@ -1896,7 +1912,7 @@
       <c r="E16" s="59">
         <v>30</v>
       </c>
-      <c r="F16" s="73" t="s">
+      <c r="F16" s="69" t="s">
         <v>16</v>
       </c>
       <c r="G16" s="58" t="s">
@@ -1909,7 +1925,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="10">
         <v>15</v>
       </c>
@@ -1922,14 +1938,14 @@
       <c r="E17" s="41">
         <v>15</v>
       </c>
-      <c r="F17" s="76">
+      <c r="F17" s="72">
         <v>0.40080579985924802</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B18" s="11">
         <v>16</v>
       </c>
@@ -1942,7 +1958,7 @@
       <c r="E18" s="38">
         <v>30</v>
       </c>
-      <c r="F18" s="72">
+      <c r="F18" s="68">
         <v>0.49419089183239701</v>
       </c>
       <c r="G18" s="20">
@@ -1958,7 +1974,7 @@
         <v>0.14756083996496799</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="12">
         <v>17</v>
       </c>
@@ -1971,14 +1987,14 @@
       <c r="E19" s="57">
         <v>15</v>
       </c>
-      <c r="F19" s="75">
+      <c r="F19" s="71">
         <v>0.31188155427417302</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B20" s="11">
         <v>18</v>
       </c>
@@ -1991,7 +2007,7 @@
       <c r="E20" s="40">
         <v>30</v>
       </c>
-      <c r="F20" s="73">
+      <c r="F20" s="69">
         <v>0.51513693782825598</v>
       </c>
       <c r="G20" s="25">
@@ -2007,7 +2023,7 @@
         <v>0.34756964057331874</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="12">
         <v>19</v>
       </c>
@@ -2020,14 +2036,14 @@
       <c r="E21" s="41">
         <v>15</v>
       </c>
-      <c r="F21" s="76">
+      <c r="F21" s="72">
         <v>0.28949053675499797</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B22" s="11">
         <v>20</v>
       </c>
@@ -2040,7 +2056,7 @@
       <c r="E22" s="38">
         <v>30</v>
       </c>
-      <c r="F22" s="72">
+      <c r="F22" s="68">
         <v>0.22319052306664899</v>
       </c>
       <c r="G22" s="20">
@@ -2056,7 +2072,7 @@
         <v>0.18288637106314115</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="12">
         <v>21</v>
       </c>
@@ -2069,14 +2085,14 @@
       <c r="E23" s="57">
         <v>15</v>
       </c>
-      <c r="F23" s="75">
+      <c r="F23" s="71">
         <v>3.4559243407891002E-2</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B24" s="13">
         <v>22</v>
       </c>
@@ -2089,7 +2105,7 @@
       <c r="E24" s="40">
         <v>30</v>
       </c>
-      <c r="F24" s="73" t="s">
+      <c r="F24" s="69" t="s">
         <v>16</v>
       </c>
       <c r="G24" s="58" t="s">
@@ -2102,11 +2118,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D25" s="45"/>
       <c r="E25" s="46"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D26" s="45"/>
       <c r="E26" s="46"/>
     </row>
@@ -2122,29 +2138,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B1:L26"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="L5" sqref="L5:O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="2"/>
-    <col min="4" max="4" width="12.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="2" customWidth="1"/>
-    <col min="7" max="9" width="7.77734375" style="2" customWidth="1"/>
-    <col min="10" max="12" width="8.88671875" style="2"/>
-    <col min="13" max="13" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="2.7890625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.89453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.89453125" style="2"/>
+    <col min="4" max="4" width="12.20703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.68359375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.68359375" style="2" customWidth="1"/>
+    <col min="7" max="9" width="7.7890625" style="2" customWidth="1"/>
+    <col min="10" max="12" width="8.89453125" style="2"/>
+    <col min="13" max="13" width="9.41796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.89453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="2:12" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
@@ -2173,7 +2189,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -2186,7 +2202,7 @@
       <c r="E3" s="37">
         <v>15</v>
       </c>
-      <c r="F3" s="74">
+      <c r="F3" s="70">
         <v>1.6037490784937101</v>
       </c>
       <c r="G3" s="18"/>
@@ -2196,7 +2212,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -2209,7 +2225,7 @@
       <c r="E4" s="42">
         <v>30</v>
       </c>
-      <c r="F4" s="74">
+      <c r="F4" s="70">
         <v>1.4997612862671901</v>
       </c>
       <c r="G4" s="55">
@@ -2225,7 +2241,7 @@
         <v>4.7385356839080489E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -2238,14 +2254,14 @@
       <c r="E5" s="39">
         <v>15</v>
       </c>
-      <c r="F5" s="75">
+      <c r="F5" s="71">
         <v>2.43401312120608</v>
       </c>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -2258,7 +2274,7 @@
       <c r="E6" s="40">
         <v>30</v>
       </c>
-      <c r="F6" s="73">
+      <c r="F6" s="69">
         <v>2.2121482351011799</v>
       </c>
       <c r="G6" s="25">
@@ -2274,7 +2290,7 @@
         <v>6.7531948824370955E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -2287,17 +2303,14 @@
       <c r="E7" s="41">
         <v>15</v>
       </c>
-      <c r="F7" s="76">
+      <c r="F7" s="72">
         <v>2.8988250174958301</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="24"/>
-      <c r="M7" s="68">
-        <v>1.19569788305308</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="11">
         <v>6</v>
       </c>
@@ -2310,17 +2323,14 @@
       <c r="E8" s="42">
         <v>30</v>
       </c>
-      <c r="F8" s="77">
+      <c r="F8" s="73">
         <v>1.77425529643583</v>
       </c>
       <c r="G8" s="28"/>
       <c r="H8" s="29"/>
       <c r="I8" s="30"/>
-      <c r="M8" s="69">
-        <v>1.2194359121409899</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -2333,17 +2343,14 @@
       <c r="E9" s="42">
         <v>15</v>
       </c>
-      <c r="F9" s="77">
+      <c r="F9" s="73">
         <v>1.2194359121409899</v>
       </c>
       <c r="G9" s="28"/>
       <c r="H9" s="29"/>
       <c r="I9" s="30"/>
-      <c r="M9" s="69">
-        <v>1.77425529643583</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -2356,7 +2363,7 @@
       <c r="E10" s="38">
         <v>30</v>
       </c>
-      <c r="F10" s="72">
+      <c r="F10" s="68">
         <v>1.19569788305308</v>
       </c>
       <c r="G10" s="20">
@@ -2371,15 +2378,8 @@
         <f>H10/G10</f>
         <v>0.44994519564122748</v>
       </c>
-      <c r="M10" s="70">
-        <v>2.8988250174958301</v>
-      </c>
-      <c r="N10" s="71">
-        <f>I10</f>
-        <v>0.44994519564122748</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="12">
         <v>9</v>
       </c>
@@ -2392,14 +2392,14 @@
       <c r="E11" s="39">
         <v>15</v>
       </c>
-      <c r="F11" s="75">
+      <c r="F11" s="71">
         <v>1.00310647552424</v>
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -2412,7 +2412,7 @@
       <c r="E12" s="40">
         <v>30</v>
       </c>
-      <c r="F12" s="73">
+      <c r="F12" s="69">
         <v>1.0972186866147799</v>
       </c>
       <c r="G12" s="25">
@@ -2428,7 +2428,7 @@
         <v>6.3368647725771346E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -2441,14 +2441,14 @@
       <c r="E13" s="41">
         <v>15</v>
       </c>
-      <c r="F13" s="76">
+      <c r="F13" s="72">
         <v>1.6656007604471099</v>
       </c>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -2461,7 +2461,7 @@
       <c r="E14" s="43">
         <v>30</v>
       </c>
-      <c r="F14" s="72" t="s">
+      <c r="F14" s="68" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="50" t="s">
@@ -2474,7 +2474,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="12">
         <v>13</v>
       </c>
@@ -2487,14 +2487,14 @@
       <c r="E15" s="39">
         <v>15</v>
       </c>
-      <c r="F15" s="75">
+      <c r="F15" s="71">
         <v>1.2018337975967099</v>
       </c>
       <c r="G15" s="23"/>
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B16" s="11">
         <v>14</v>
       </c>
@@ -2507,7 +2507,7 @@
       <c r="E16" s="59">
         <v>30</v>
       </c>
-      <c r="F16" s="73" t="s">
+      <c r="F16" s="69" t="s">
         <v>16</v>
       </c>
       <c r="G16" s="58" t="s">
@@ -2520,7 +2520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="10">
         <v>15</v>
       </c>
@@ -2533,14 +2533,14 @@
       <c r="E17" s="51">
         <v>15</v>
       </c>
-      <c r="F17" s="74">
+      <c r="F17" s="70">
         <v>0.248726053876346</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B18" s="11">
         <v>16</v>
       </c>
@@ -2553,7 +2553,7 @@
       <c r="E18" s="42">
         <v>30</v>
       </c>
-      <c r="F18" s="74">
+      <c r="F18" s="70">
         <v>0.55572193204928499</v>
       </c>
       <c r="G18" s="55">
@@ -2569,7 +2569,7 @@
         <v>0.53969646527891901</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="12">
         <v>17</v>
       </c>
@@ -2582,14 +2582,14 @@
       <c r="E19" s="57">
         <v>15</v>
       </c>
-      <c r="F19" s="75">
+      <c r="F19" s="71">
         <v>0.33417300109709502</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B20" s="11">
         <v>18</v>
       </c>
@@ -2602,7 +2602,7 @@
       <c r="E20" s="49">
         <v>30</v>
       </c>
-      <c r="F20" s="78">
+      <c r="F20" s="74">
         <v>0.63737196876332802</v>
       </c>
       <c r="G20" s="61">
@@ -2618,7 +2618,7 @@
         <v>0.44134662364904237</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="12">
         <v>19</v>
       </c>
@@ -2631,14 +2631,14 @@
       <c r="E21" s="41">
         <v>15</v>
       </c>
-      <c r="F21" s="76">
+      <c r="F21" s="72">
         <v>0.57148050234214598</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B22" s="11">
         <v>20</v>
       </c>
@@ -2651,7 +2651,7 @@
       <c r="E22" s="38">
         <v>30</v>
       </c>
-      <c r="F22" s="72">
+      <c r="F22" s="68">
         <v>0.72410818061410198</v>
       </c>
       <c r="G22" s="20">
@@ -2667,7 +2667,7 @@
         <v>0.16660236033646106</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="12">
         <v>21</v>
       </c>
@@ -2680,14 +2680,14 @@
       <c r="E23" s="49">
         <v>15</v>
       </c>
-      <c r="F23" s="78">
+      <c r="F23" s="74">
         <v>3.4042514760134999E-2</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B24" s="13">
         <v>22</v>
       </c>
@@ -2700,7 +2700,7 @@
       <c r="E24" s="40">
         <v>30</v>
       </c>
-      <c r="F24" s="73" t="s">
+      <c r="F24" s="69" t="s">
         <v>16</v>
       </c>
       <c r="G24" s="58" t="s">
@@ -2713,11 +2713,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D25" s="45"/>
       <c r="E25" s="46"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D26" s="45"/>
       <c r="E26" s="46"/>
     </row>
@@ -2733,27 +2733,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="L5" sqref="L5:P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="2"/>
-    <col min="4" max="4" width="12.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="2" customWidth="1"/>
-    <col min="7" max="9" width="7.77734375" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="2.7890625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.89453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.89453125" style="2"/>
+    <col min="4" max="4" width="12.20703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.68359375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.68359375" style="2" customWidth="1"/>
+    <col min="7" max="9" width="7.7890625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.89453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="2:12" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
@@ -2782,7 +2782,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -2795,7 +2795,7 @@
       <c r="E3" s="37">
         <v>15</v>
       </c>
-      <c r="F3" s="76">
+      <c r="F3" s="72">
         <v>8.4540385981037893</v>
       </c>
       <c r="G3" s="18"/>
@@ -2805,7 +2805,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -2818,7 +2818,7 @@
       <c r="E4" s="38">
         <v>30</v>
       </c>
-      <c r="F4" s="72">
+      <c r="F4" s="68">
         <v>8.1392711878697899</v>
       </c>
       <c r="G4" s="20">
@@ -2834,7 +2834,7 @@
         <v>2.6826977033976924E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -2847,14 +2847,14 @@
       <c r="E5" s="39">
         <v>15</v>
       </c>
-      <c r="F5" s="75">
+      <c r="F5" s="71">
         <v>6.8658138939520299</v>
       </c>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -2867,7 +2867,7 @@
       <c r="E6" s="40">
         <v>30</v>
       </c>
-      <c r="F6" s="73">
+      <c r="F6" s="69">
         <v>9.5193853680806395</v>
       </c>
       <c r="G6" s="25">
@@ -2883,7 +2883,7 @@
         <v>0.22903088985525652</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -2896,17 +2896,14 @@
       <c r="E7" s="41">
         <v>15</v>
       </c>
-      <c r="F7" s="76">
+      <c r="F7" s="72">
         <v>8.12727339067294</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="24"/>
-      <c r="M7" s="68">
-        <v>5.70671799511498</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="11">
         <v>6</v>
       </c>
@@ -2919,17 +2916,14 @@
       <c r="E8" s="42">
         <v>30</v>
       </c>
-      <c r="F8" s="77">
+      <c r="F8" s="73">
         <v>8.4269394103516007</v>
       </c>
       <c r="G8" s="28"/>
       <c r="H8" s="29"/>
       <c r="I8" s="30"/>
-      <c r="M8" s="69">
-        <v>6.5621740368524604</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -2942,17 +2936,14 @@
       <c r="E9" s="42">
         <v>15</v>
       </c>
-      <c r="F9" s="77">
+      <c r="F9" s="73">
         <v>5.70671799511498</v>
       </c>
       <c r="G9" s="28"/>
       <c r="H9" s="29"/>
       <c r="I9" s="30"/>
-      <c r="M9" s="69">
-        <v>8.12727339067294</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -2965,7 +2956,7 @@
       <c r="E10" s="38">
         <v>30</v>
       </c>
-      <c r="F10" s="72">
+      <c r="F10" s="68">
         <v>6.5621740368524604</v>
       </c>
       <c r="G10" s="20">
@@ -2980,15 +2971,8 @@
         <f>H10/G10</f>
         <v>0.17919322511738361</v>
       </c>
-      <c r="M10" s="70">
-        <v>8.4269394103516007</v>
-      </c>
-      <c r="N10" s="71">
-        <f>I10</f>
-        <v>0.17919322511738361</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="12">
         <v>9</v>
       </c>
@@ -3001,14 +2985,14 @@
       <c r="E11" s="39">
         <v>15</v>
       </c>
-      <c r="F11" s="75">
+      <c r="F11" s="71">
         <v>18.206022025999399</v>
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -3021,7 +3005,7 @@
       <c r="E12" s="40">
         <v>30</v>
       </c>
-      <c r="F12" s="73">
+      <c r="F12" s="69">
         <v>17.605520191289099</v>
       </c>
       <c r="G12" s="25">
@@ -3037,7 +3021,7 @@
         <v>2.3714081726065751E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -3050,14 +3034,14 @@
       <c r="E13" s="41">
         <v>15</v>
       </c>
-      <c r="F13" s="76">
+      <c r="F13" s="72">
         <v>11.614496160065499</v>
       </c>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -3070,7 +3054,7 @@
       <c r="E14" s="43">
         <v>30</v>
       </c>
-      <c r="F14" s="72" t="s">
+      <c r="F14" s="68" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="50" t="s">
@@ -3083,7 +3067,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="12">
         <v>13</v>
       </c>
@@ -3096,14 +3080,14 @@
       <c r="E15" s="39">
         <v>15</v>
       </c>
-      <c r="F15" s="75">
+      <c r="F15" s="71">
         <v>3.53592699984979</v>
       </c>
       <c r="G15" s="23"/>
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B16" s="11">
         <v>14</v>
       </c>
@@ -3116,7 +3100,7 @@
       <c r="E16" s="59">
         <v>30</v>
       </c>
-      <c r="F16" s="73" t="s">
+      <c r="F16" s="69" t="s">
         <v>16</v>
       </c>
       <c r="G16" s="58" t="s">
@@ -3129,7 +3113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="10">
         <v>15</v>
       </c>
@@ -3142,14 +3126,14 @@
       <c r="E17" s="41">
         <v>15</v>
       </c>
-      <c r="F17" s="76">
+      <c r="F17" s="72">
         <v>19.9912607666577</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B18" s="11">
         <v>16</v>
       </c>
@@ -3162,7 +3146,7 @@
       <c r="E18" s="38">
         <v>30</v>
       </c>
-      <c r="F18" s="72">
+      <c r="F18" s="68">
         <v>20.118165863553902</v>
       </c>
       <c r="G18" s="20">
@@ -3178,7 +3162,7 @@
         <v>4.4745319054174133E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="12">
         <v>17</v>
       </c>
@@ -3191,14 +3175,14 @@
       <c r="E19" s="57">
         <v>15</v>
       </c>
-      <c r="F19" s="75">
+      <c r="F19" s="71">
         <v>1.4138148878347501</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B20" s="11">
         <v>18</v>
       </c>
@@ -3211,7 +3195,7 @@
       <c r="E20" s="40">
         <v>30</v>
       </c>
-      <c r="F20" s="73">
+      <c r="F20" s="69">
         <v>3.6219553113350398</v>
       </c>
       <c r="G20" s="25">
@@ -3227,7 +3211,7 @@
         <v>0.62012006327318359</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="12">
         <v>19</v>
       </c>
@@ -3240,14 +3224,14 @@
       <c r="E21" s="41">
         <v>15</v>
       </c>
-      <c r="F21" s="76">
+      <c r="F21" s="72">
         <v>12.116454971455999</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B22" s="11">
         <v>20</v>
       </c>
@@ -3260,7 +3244,7 @@
       <c r="E22" s="38">
         <v>30</v>
       </c>
-      <c r="F22" s="72">
+      <c r="F22" s="68">
         <v>0.94206422210385099</v>
       </c>
       <c r="G22" s="20">
@@ -3276,7 +3260,7 @@
         <v>1.2101659242331178</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="12">
         <v>21</v>
       </c>
@@ -3289,14 +3273,14 @@
       <c r="E23" s="57">
         <v>15</v>
       </c>
-      <c r="F23" s="75">
+      <c r="F23" s="71">
         <v>0.18225239663838</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B24" s="13">
         <v>22</v>
       </c>
@@ -3309,7 +3293,7 @@
       <c r="E24" s="40">
         <v>30</v>
       </c>
-      <c r="F24" s="73" t="s">
+      <c r="F24" s="69" t="s">
         <v>16</v>
       </c>
       <c r="G24" s="58" t="s">
@@ -3322,15 +3306,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D25" s="45"/>
       <c r="E25" s="46"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D26" s="45"/>
       <c r="E26" s="46"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D27" s="45"/>
       <c r="E27" s="46"/>
     </row>
@@ -3346,29 +3330,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="B1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5:O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="2"/>
-    <col min="4" max="4" width="12.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="2" customWidth="1"/>
-    <col min="7" max="9" width="7.77734375" style="2" customWidth="1"/>
-    <col min="10" max="12" width="8.88671875" style="2"/>
-    <col min="13" max="13" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="2.7890625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.89453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.89453125" style="2"/>
+    <col min="4" max="4" width="12.20703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.68359375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.68359375" style="2" customWidth="1"/>
+    <col min="7" max="9" width="7.7890625" style="2" customWidth="1"/>
+    <col min="10" max="12" width="8.89453125" style="2"/>
+    <col min="13" max="13" width="9.41796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.89453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="2:12" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
@@ -3397,7 +3381,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -3410,7 +3394,7 @@
       <c r="E3" s="37">
         <v>15</v>
       </c>
-      <c r="F3" s="76">
+      <c r="F3" s="72">
         <v>0.43117404664541698</v>
       </c>
       <c r="G3" s="18"/>
@@ -3420,7 +3404,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -3433,7 +3417,7 @@
       <c r="E4" s="38">
         <v>30</v>
       </c>
-      <c r="F4" s="72">
+      <c r="F4" s="68">
         <v>0.397888334964139</v>
       </c>
       <c r="G4" s="20">
@@ -3449,7 +3433,7 @@
         <v>5.677872490308309E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -3462,14 +3446,14 @@
       <c r="E5" s="39">
         <v>15</v>
       </c>
-      <c r="F5" s="75">
+      <c r="F5" s="71">
         <v>0.37728316960245101</v>
       </c>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -3482,7 +3466,7 @@
       <c r="E6" s="40">
         <v>30</v>
       </c>
-      <c r="F6" s="73">
+      <c r="F6" s="69">
         <v>0.38849744237329698</v>
       </c>
       <c r="G6" s="25">
@@ -3498,7 +3482,7 @@
         <v>2.0710078574284849E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -3511,17 +3495,14 @@
       <c r="E7" s="41">
         <v>15</v>
       </c>
-      <c r="F7" s="76">
+      <c r="F7" s="72">
         <v>0.38037299526942198</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="24"/>
-      <c r="M7" s="68">
-        <v>0.37378688770538299</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="11">
         <v>6</v>
       </c>
@@ -3534,17 +3515,14 @@
       <c r="E8" s="42">
         <v>30</v>
       </c>
-      <c r="F8" s="77">
+      <c r="F8" s="73">
         <v>0.39845264310084899</v>
       </c>
       <c r="G8" s="28"/>
       <c r="H8" s="29"/>
       <c r="I8" s="30"/>
-      <c r="M8" s="69">
-        <v>0.38037299526942198</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -3557,17 +3535,14 @@
       <c r="E9" s="42">
         <v>15</v>
       </c>
-      <c r="F9" s="77">
+      <c r="F9" s="73">
         <v>0.37378688770538299</v>
       </c>
       <c r="G9" s="28"/>
       <c r="H9" s="29"/>
       <c r="I9" s="30"/>
-      <c r="M9" s="69">
-        <v>0.384164974612001</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -3580,7 +3555,7 @@
       <c r="E10" s="38">
         <v>30</v>
       </c>
-      <c r="F10" s="72">
+      <c r="F10" s="68">
         <v>0.384164974612001</v>
       </c>
       <c r="G10" s="20">
@@ -3595,15 +3570,8 @@
         <f>H10/G10</f>
         <v>2.7142022318979806E-2</v>
       </c>
-      <c r="M10" s="70">
-        <v>0.39845264310084899</v>
-      </c>
-      <c r="N10" s="71">
-        <f>I10</f>
-        <v>2.7142022318979806E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="12">
         <v>9</v>
       </c>
@@ -3616,14 +3584,14 @@
       <c r="E11" s="48">
         <v>15</v>
       </c>
-      <c r="F11" s="78">
+      <c r="F11" s="74">
         <v>0.26530110709080001</v>
       </c>
       <c r="G11" s="52"/>
       <c r="H11" s="52"/>
       <c r="I11" s="53"/>
     </row>
-    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -3636,7 +3604,7 @@
       <c r="E12" s="49">
         <v>30</v>
       </c>
-      <c r="F12" s="78">
+      <c r="F12" s="74">
         <v>0.26364307110920399</v>
       </c>
       <c r="G12" s="61">
@@ -3652,7 +3620,7 @@
         <v>4.4330140470684428E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -3665,14 +3633,14 @@
       <c r="E13" s="41">
         <v>15</v>
       </c>
-      <c r="F13" s="76">
+      <c r="F13" s="72">
         <v>0.43619881125905602</v>
       </c>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -3685,7 +3653,7 @@
       <c r="E14" s="43">
         <v>30</v>
       </c>
-      <c r="F14" s="72" t="s">
+      <c r="F14" s="68" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="50" t="s">
@@ -3698,7 +3666,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="12">
         <v>13</v>
       </c>
@@ -3711,14 +3679,14 @@
       <c r="E15" s="39">
         <v>15</v>
       </c>
-      <c r="F15" s="75">
+      <c r="F15" s="71">
         <v>0.262636074968565</v>
       </c>
       <c r="G15" s="23"/>
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B16" s="11">
         <v>14</v>
       </c>
@@ -3731,7 +3699,7 @@
       <c r="E16" s="59">
         <v>30</v>
       </c>
-      <c r="F16" s="73" t="s">
+      <c r="F16" s="69" t="s">
         <v>16</v>
       </c>
       <c r="G16" s="58" t="s">
@@ -3744,7 +3712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="10">
         <v>15</v>
       </c>
@@ -3757,14 +3725,14 @@
       <c r="E17" s="51">
         <v>15</v>
       </c>
-      <c r="F17" s="74">
+      <c r="F17" s="70">
         <v>0.26254378888276098</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B18" s="11">
         <v>16</v>
       </c>
@@ -3777,7 +3745,7 @@
       <c r="E18" s="42">
         <v>30</v>
       </c>
-      <c r="F18" s="74">
+      <c r="F18" s="70">
         <v>0.26250488812556</v>
       </c>
       <c r="G18" s="55">
@@ -3793,7 +3761,7 @@
         <v>1.0477881543035028E-4</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="12">
         <v>17</v>
       </c>
@@ -3806,14 +3774,14 @@
       <c r="E19" s="57">
         <v>15</v>
       </c>
-      <c r="F19" s="75">
+      <c r="F19" s="71">
         <v>0.43347359394512402</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B20" s="11">
         <v>18</v>
       </c>
@@ -3826,7 +3794,7 @@
       <c r="E20" s="40">
         <v>30</v>
       </c>
-      <c r="F20" s="73">
+      <c r="F20" s="69">
         <v>0.30272722907173599</v>
       </c>
       <c r="G20" s="25">
@@ -3842,7 +3810,7 @@
         <v>0.25115875540211463</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="12">
         <v>19</v>
       </c>
@@ -3855,14 +3823,14 @@
       <c r="E21" s="41">
         <v>15</v>
       </c>
-      <c r="F21" s="76">
+      <c r="F21" s="72">
         <v>0.26256077846496401</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B22" s="11">
         <v>20</v>
       </c>
@@ -3875,7 +3843,7 @@
       <c r="E22" s="38">
         <v>30</v>
       </c>
-      <c r="F22" s="72">
+      <c r="F22" s="68">
         <v>0.37616392381888403</v>
       </c>
       <c r="G22" s="20">
@@ -3891,7 +3859,7 @@
         <v>0.25153107170162187</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="12">
         <v>21</v>
       </c>
@@ -3904,14 +3872,14 @@
       <c r="E23" s="57">
         <v>15</v>
       </c>
-      <c r="F23" s="75">
+      <c r="F23" s="71">
         <v>0.27895426965193099</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B24" s="13">
         <v>22</v>
       </c>
@@ -3924,7 +3892,7 @@
       <c r="E24" s="40">
         <v>30</v>
       </c>
-      <c r="F24" s="73" t="s">
+      <c r="F24" s="69" t="s">
         <v>16</v>
       </c>
       <c r="G24" s="58" t="s">
@@ -3937,11 +3905,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D25" s="45"/>
       <c r="E25" s="46"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D26" s="45"/>
       <c r="E26" s="46"/>
     </row>
@@ -3957,27 +3925,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="B1:P25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4:P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="2"/>
-    <col min="4" max="4" width="12.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="2" customWidth="1"/>
-    <col min="7" max="9" width="7.77734375" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="2.7890625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.89453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.89453125" style="2"/>
+    <col min="4" max="4" width="12.20703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.68359375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.68359375" style="2" customWidth="1"/>
+    <col min="7" max="9" width="7.7890625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.89453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:14" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="2:16" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
@@ -4006,7 +3974,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -4019,7 +3987,7 @@
       <c r="E3" s="37">
         <v>15</v>
       </c>
-      <c r="F3" s="74">
+      <c r="F3" s="70">
         <v>4.7927253180343303</v>
       </c>
       <c r="G3" s="18"/>
@@ -4029,7 +3997,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -4042,7 +4010,7 @@
       <c r="E4" s="42">
         <v>30</v>
       </c>
-      <c r="F4" s="74">
+      <c r="F4" s="70">
         <v>4.9929511217925802</v>
       </c>
       <c r="G4" s="55">
@@ -4057,8 +4025,13 @@
         <f>H4/G4</f>
         <v>2.8936379508679045E-2</v>
       </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -4071,14 +4044,19 @@
       <c r="E5" s="39">
         <v>15</v>
       </c>
-      <c r="F5" s="75">
+      <c r="F5" s="71">
         <v>4.7686734078400601</v>
       </c>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="24"/>
-    </row>
-    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="2:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -4091,7 +4069,7 @@
       <c r="E6" s="40">
         <v>30</v>
       </c>
-      <c r="F6" s="73">
+      <c r="F6" s="69">
         <v>4.9077985848138601</v>
       </c>
       <c r="G6" s="25">
@@ -4106,8 +4084,13 @@
         <f>H6/G6</f>
         <v>2.0333104078973579E-2</v>
       </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -4120,17 +4103,19 @@
       <c r="E7" s="41">
         <v>15</v>
       </c>
-      <c r="F7" s="76">
+      <c r="F7" s="72">
         <v>5.4147152806680898</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="24"/>
-      <c r="M7" s="68">
-        <v>5.4147152806680898</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="11">
         <v>6</v>
       </c>
@@ -4143,17 +4128,19 @@
       <c r="E8" s="42">
         <v>30</v>
       </c>
-      <c r="F8" s="77">
+      <c r="F8" s="73">
         <v>5.3848833614323004</v>
       </c>
       <c r="G8" s="28"/>
       <c r="H8" s="29"/>
       <c r="I8" s="30"/>
-      <c r="M8" s="69">
-        <v>5.3848833614323004</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -4166,17 +4153,19 @@
       <c r="E9" s="42">
         <v>15</v>
       </c>
-      <c r="F9" s="77">
+      <c r="F9" s="73">
         <v>5.3219131078384603</v>
       </c>
       <c r="G9" s="28"/>
       <c r="H9" s="29"/>
       <c r="I9" s="30"/>
-      <c r="M9" s="69">
-        <v>5.3219131078384603</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="2:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -4189,7 +4178,7 @@
       <c r="E10" s="38">
         <v>30</v>
       </c>
-      <c r="F10" s="72">
+      <c r="F10" s="68">
         <v>5.24076159044085</v>
       </c>
       <c r="G10" s="20">
@@ -4204,15 +4193,13 @@
         <f>H10/G10</f>
         <v>1.4411452912174955E-2</v>
       </c>
-      <c r="M10" s="70">
-        <v>5.24076159044085</v>
-      </c>
-      <c r="N10" s="71">
-        <f>I10</f>
-        <v>1.4411452912174955E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="12">
         <v>9</v>
       </c>
@@ -4225,14 +4212,19 @@
       <c r="E11" s="39">
         <v>15</v>
       </c>
-      <c r="F11" s="75">
+      <c r="F11" s="71">
         <v>5.1851464382301202</v>
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
       <c r="I11" s="24"/>
-    </row>
-    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="2:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -4245,7 +4237,7 @@
       <c r="E12" s="40">
         <v>30</v>
       </c>
-      <c r="F12" s="73">
+      <c r="F12" s="69">
         <v>5.2284692910135604</v>
       </c>
       <c r="G12" s="25">
@@ -4260,8 +4252,13 @@
         <f>H12/G12</f>
         <v>5.883428730232571E-3</v>
       </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -4274,14 +4271,19 @@
       <c r="E13" s="41">
         <v>15</v>
       </c>
-      <c r="F13" s="76">
+      <c r="F13" s="72">
         <v>3.6676623808811999</v>
       </c>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
-    </row>
-    <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="2:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -4294,7 +4296,7 @@
       <c r="E14" s="43">
         <v>30</v>
       </c>
-      <c r="F14" s="72" t="s">
+      <c r="F14" s="68" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="50" t="s">
@@ -4307,7 +4309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="12">
         <v>13</v>
       </c>
@@ -4320,14 +4322,14 @@
       <c r="E15" s="48">
         <v>15</v>
       </c>
-      <c r="F15" s="78">
+      <c r="F15" s="74">
         <v>1.3169165514435499</v>
       </c>
       <c r="G15" s="52"/>
       <c r="H15" s="52"/>
       <c r="I15" s="53"/>
     </row>
-    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B16" s="11">
         <v>14</v>
       </c>
@@ -4340,7 +4342,7 @@
       <c r="E16" s="59">
         <v>30</v>
       </c>
-      <c r="F16" s="73" t="s">
+      <c r="F16" s="69" t="s">
         <v>16</v>
       </c>
       <c r="G16" s="58" t="s">
@@ -4353,7 +4355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="10">
         <v>15</v>
       </c>
@@ -4366,14 +4368,14 @@
       <c r="E17" s="41">
         <v>15</v>
       </c>
-      <c r="F17" s="76">
+      <c r="F17" s="72">
         <v>5.5439082357326503</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B18" s="11">
         <v>16</v>
       </c>
@@ -4386,7 +4388,7 @@
       <c r="E18" s="38">
         <v>30</v>
       </c>
-      <c r="F18" s="72">
+      <c r="F18" s="68">
         <v>7.62086262055149</v>
       </c>
       <c r="G18" s="20">
@@ -4402,7 +4404,7 @@
         <v>0.2231149399793004</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="12">
         <v>17</v>
       </c>
@@ -4415,14 +4417,14 @@
       <c r="E19" s="57">
         <v>15</v>
       </c>
-      <c r="F19" s="75">
+      <c r="F19" s="71">
         <v>4.3589496333595399</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B20" s="11">
         <v>18</v>
       </c>
@@ -4435,7 +4437,7 @@
       <c r="E20" s="40">
         <v>30</v>
       </c>
-      <c r="F20" s="73">
+      <c r="F20" s="69">
         <v>7.2509901643550201</v>
       </c>
       <c r="G20" s="25">
@@ -4451,7 +4453,7 @@
         <v>0.35228114987052844</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="12">
         <v>19</v>
       </c>
@@ -4464,14 +4466,14 @@
       <c r="E21" s="41">
         <v>15</v>
       </c>
-      <c r="F21" s="76">
+      <c r="F21" s="72">
         <v>3.9892512275732099</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B22" s="11">
         <v>20</v>
       </c>
@@ -4484,7 +4486,7 @@
       <c r="E22" s="38">
         <v>30</v>
       </c>
-      <c r="F22" s="72">
+      <c r="F22" s="68">
         <v>3.1814215963461701</v>
       </c>
       <c r="G22" s="20">
@@ -4500,7 +4502,7 @@
         <v>0.1593216771454497</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="12">
         <v>21</v>
       </c>
@@ -4513,14 +4515,14 @@
       <c r="E23" s="49">
         <v>15</v>
       </c>
-      <c r="F23" s="78">
+      <c r="F23" s="74">
         <v>0.53935270821925096</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B24" s="13">
         <v>22</v>
       </c>
@@ -4533,7 +4535,7 @@
       <c r="E24" s="40">
         <v>30</v>
       </c>
-      <c r="F24" s="73" t="s">
+      <c r="F24" s="69" t="s">
         <v>16</v>
       </c>
       <c r="G24" s="58" t="s">
@@ -4546,7 +4548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D25" s="45"/>
       <c r="E25" s="46"/>
     </row>
@@ -4559,27 +4561,27 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="B1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="2"/>
-    <col min="4" max="4" width="12.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="2" customWidth="1"/>
-    <col min="7" max="9" width="7.77734375" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="2.7890625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.89453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.89453125" style="2"/>
+    <col min="4" max="4" width="12.20703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.68359375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.68359375" style="2" customWidth="1"/>
+    <col min="7" max="9" width="7.7890625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.89453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="2:12" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
@@ -4608,7 +4610,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -4621,7 +4623,7 @@
       <c r="E3" s="37">
         <v>15</v>
       </c>
-      <c r="F3" s="74">
+      <c r="F3" s="70">
         <v>0.76186897132864095</v>
       </c>
       <c r="G3" s="18"/>
@@ -4631,7 +4633,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -4644,7 +4646,7 @@
       <c r="E4" s="42">
         <v>30</v>
       </c>
-      <c r="F4" s="74">
+      <c r="F4" s="70">
         <v>0.78514709098936497</v>
       </c>
       <c r="G4" s="55">
@@ -4660,7 +4662,7 @@
         <v>2.1279825938854784E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -4673,14 +4675,14 @@
       <c r="E5" s="39">
         <v>15</v>
       </c>
-      <c r="F5" s="75">
+      <c r="F5" s="71">
         <v>0.79522786376675303</v>
       </c>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -4693,7 +4695,7 @@
       <c r="E6" s="40">
         <v>30</v>
       </c>
-      <c r="F6" s="73">
+      <c r="F6" s="69">
         <v>0.78982757506022905</v>
       </c>
       <c r="G6" s="25">
@@ -4709,7 +4711,7 @@
         <v>4.8182299132378259E-3</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -4722,17 +4724,14 @@
       <c r="E7" s="41">
         <v>15</v>
       </c>
-      <c r="F7" s="76">
+      <c r="F7" s="72">
         <v>0.81142827210842305</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="24"/>
-      <c r="M7" s="76">
-        <v>0.81142827200000001</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="11">
         <v>6</v>
       </c>
@@ -4745,17 +4744,14 @@
       <c r="E8" s="42">
         <v>30</v>
       </c>
-      <c r="F8" s="77">
+      <c r="F8" s="73">
         <v>0.77528859277047801</v>
       </c>
       <c r="G8" s="28"/>
       <c r="H8" s="29"/>
       <c r="I8" s="30"/>
-      <c r="M8" s="77">
-        <v>0.77528859299999997</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -4768,17 +4764,14 @@
       <c r="E9" s="42">
         <v>15</v>
       </c>
-      <c r="F9" s="77">
+      <c r="F9" s="73">
         <v>0.850827072994217</v>
       </c>
       <c r="G9" s="28"/>
       <c r="H9" s="29"/>
       <c r="I9" s="30"/>
-      <c r="M9" s="77">
-        <v>0.85082707300000004</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -4791,7 +4784,7 @@
       <c r="E10" s="38">
         <v>30</v>
       </c>
-      <c r="F10" s="72">
+      <c r="F10" s="68">
         <v>0.82117144427272404</v>
       </c>
       <c r="G10" s="20">
@@ -4806,15 +4799,8 @@
         <f>H10/G10</f>
         <v>3.8236181592972401E-2</v>
       </c>
-      <c r="M10" s="72">
-        <v>0.82117144399999997</v>
-      </c>
-      <c r="N10" s="71">
-        <f>I10</f>
-        <v>3.8236181592972401E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="12">
         <v>9</v>
       </c>
@@ -4827,14 +4813,14 @@
       <c r="E11" s="39">
         <v>15</v>
       </c>
-      <c r="F11" s="75">
+      <c r="F11" s="71">
         <v>0.74996612541989005</v>
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -4847,7 +4833,7 @@
       <c r="E12" s="40">
         <v>30</v>
       </c>
-      <c r="F12" s="73">
+      <c r="F12" s="69">
         <v>0.76237080581552596</v>
       </c>
       <c r="G12" s="25">
@@ -4863,7 +4849,7 @@
         <v>1.1599840544845606E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -4876,14 +4862,14 @@
       <c r="E13" s="41">
         <v>15</v>
       </c>
-      <c r="F13" s="76">
+      <c r="F13" s="72">
         <v>0.72943610951139104</v>
       </c>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -4896,7 +4882,7 @@
       <c r="E14" s="43">
         <v>30</v>
       </c>
-      <c r="F14" s="72" t="s">
+      <c r="F14" s="68" t="s">
         <v>17</v>
       </c>
       <c r="G14" s="50" t="s">
@@ -4909,7 +4895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="12">
         <v>13</v>
       </c>
@@ -4922,14 +4908,14 @@
       <c r="E15" s="39">
         <v>15</v>
       </c>
-      <c r="F15" s="75">
+      <c r="F15" s="71">
         <v>0.82088178902345099</v>
       </c>
       <c r="G15" s="23"/>
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B16" s="11">
         <v>14</v>
       </c>
@@ -4942,7 +4928,7 @@
       <c r="E16" s="59">
         <v>30</v>
       </c>
-      <c r="F16" s="73" t="s">
+      <c r="F16" s="69" t="s">
         <v>17</v>
       </c>
       <c r="G16" s="58" t="s">
@@ -4955,7 +4941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="10">
         <v>15</v>
       </c>
@@ -4968,14 +4954,14 @@
       <c r="E17" s="51">
         <v>15</v>
       </c>
-      <c r="F17" s="74">
+      <c r="F17" s="70">
         <v>0.75261688024566598</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B18" s="11">
         <v>16</v>
       </c>
@@ -4988,7 +4974,7 @@
       <c r="E18" s="42">
         <v>30</v>
       </c>
-      <c r="F18" s="74">
+      <c r="F18" s="70">
         <v>0.79435293357597203</v>
       </c>
       <c r="G18" s="55">
@@ -5004,7 +4990,7 @@
         <v>3.8154391981207014E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="12">
         <v>17</v>
       </c>
@@ -5017,14 +5003,14 @@
       <c r="E19" s="57">
         <v>15</v>
       </c>
-      <c r="F19" s="75">
+      <c r="F19" s="71">
         <v>0.94578732603498405</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B20" s="11">
         <v>18</v>
       </c>
@@ -5037,7 +5023,7 @@
       <c r="E20" s="40">
         <v>30</v>
       </c>
-      <c r="F20" s="73">
+      <c r="F20" s="69">
         <v>0.968625246038328</v>
       </c>
       <c r="G20" s="25">
@@ -5053,7 +5039,7 @@
         <v>1.6870812841634417E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="12">
         <v>19</v>
       </c>
@@ -5066,14 +5052,14 @@
       <c r="E21" s="41">
         <v>15</v>
       </c>
-      <c r="F21" s="76">
+      <c r="F21" s="72">
         <v>0.78454965510937802</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B22" s="11">
         <v>20</v>
       </c>
@@ -5086,7 +5072,7 @@
       <c r="E22" s="38">
         <v>30</v>
       </c>
-      <c r="F22" s="72">
+      <c r="F22" s="68">
         <v>0.97492797526238795</v>
       </c>
       <c r="G22" s="20">
@@ -5102,7 +5088,7 @@
         <v>0.15302019059219743</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="12">
         <v>21</v>
       </c>
@@ -5115,14 +5101,14 @@
       <c r="E23" s="57">
         <v>15</v>
       </c>
-      <c r="F23" s="75">
+      <c r="F23" s="71">
         <v>0.962410634731658</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B24" s="13">
         <v>22</v>
       </c>
@@ -5135,7 +5121,7 @@
       <c r="E24" s="40">
         <v>30</v>
       </c>
-      <c r="F24" s="73" t="s">
+      <c r="F24" s="69" t="s">
         <v>17</v>
       </c>
       <c r="G24" s="58" t="s">
@@ -5148,11 +5134,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D25" s="45"/>
       <c r="E25" s="46"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D26" s="45"/>
       <c r="E26" s="46"/>
     </row>

</xml_diff>